<commit_message>
update api brand and influencer
</commit_message>
<xml_diff>
--- a/src/main/resources/template/InfluencerImport.xlsx
+++ b/src/main/resources/template/InfluencerImport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\IdeaProject\Halago-Dainv\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ideiaProject\Halago-Dainv\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94ABB07-BF21-4FA0-AFA0-CDD967B8A6DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Influencer" sheetId="1" r:id="rId1"/>
@@ -90,16 +89,16 @@
     <t>Follower Facebook</t>
   </si>
   <si>
-    <t>Chi phí Fb</t>
-  </si>
-  <si>
     <t>Tỉnh</t>
+  </si>
+  <si>
+    <t>Chi phí Facebook</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,43 +413,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="14" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" style="2" customWidth="1"/>
     <col min="8" max="8" width="13" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" style="2" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="16.42578125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="15.140625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="13.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22.5546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="14.5546875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="17.33203125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="16.44140625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="15.109375" style="2" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +478,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -491,7 +490,7 @@
         <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>10</v>

</xml_diff>